<commit_message>
test matrix & Hughes stitch
</commit_message>
<xml_diff>
--- a/Opt_Test_Matrix.xlsx
+++ b/Opt_Test_Matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rthill\Documents\MS-Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE6C4CF0-C0FA-452B-9601-3138B91FE95A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FB7BEEE-CF77-4187-98A6-1A85BE4315C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{ACE28608-3E68-4E86-80D4-7B51E677897B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t xml:space="preserve">Structural Design Weight and Cost Tradeoffs for Attritable Vessels </t>
   </si>
@@ -145,12 +145,15 @@
       <t>Bot_Plate</t>
     </r>
   </si>
+  <si>
+    <t>*run these 4 cases first before continuing</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -171,6 +174,13 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -347,52 +357,55 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -823,8 +836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5177AB5A-2235-443C-BFC0-3BF5F1CC385F}">
   <dimension ref="B2:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -836,337 +849,398 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="15.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
     </row>
     <row r="3" spans="2:9" ht="15.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
     </row>
     <row r="4" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="5" spans="2:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="2:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C6" s="7"/>
-      <c r="D6" s="8">
+      <c r="C6" s="13"/>
+      <c r="D6" s="5">
         <v>1</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="F6" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="G6" s="7">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="C7" s="13"/>
+      <c r="D7" s="8">
+        <v>2</v>
+      </c>
+      <c r="E7" s="9">
+        <v>1.5</v>
+      </c>
+      <c r="F7" s="10">
+        <v>1.4</v>
+      </c>
+      <c r="G7" s="10">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="C8" s="13"/>
+      <c r="D8" s="8">
         <v>3</v>
       </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-    </row>
-    <row r="7" spans="2:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C7" s="7"/>
-      <c r="D7" s="11">
-        <v>2</v>
-      </c>
-      <c r="E7" s="12">
-        <v>3</v>
-      </c>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-    </row>
-    <row r="8" spans="2:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C8" s="7"/>
-      <c r="D8" s="11">
-        <v>3</v>
-      </c>
-      <c r="E8" s="12">
-        <v>2.5</v>
-      </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="E8" s="9">
+        <v>1.25</v>
+      </c>
+      <c r="F8" s="10">
+        <v>1.3</v>
+      </c>
+      <c r="G8" s="10">
+        <v>1.2</v>
+      </c>
     </row>
     <row r="9" spans="2:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C9" s="7"/>
-      <c r="D9" s="11">
+      <c r="C9" s="13"/>
+      <c r="D9" s="8">
         <v>4</v>
       </c>
-      <c r="E9" s="12">
-        <v>2.5</v>
-      </c>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="E9" s="9">
+        <v>1.25</v>
+      </c>
+      <c r="F9" s="10">
+        <v>1.2</v>
+      </c>
+      <c r="G9" s="10">
+        <v>1.1000000000000001</v>
+      </c>
     </row>
     <row r="10" spans="2:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C10" s="7"/>
-      <c r="D10" s="11">
+      <c r="C10" s="13"/>
+      <c r="D10" s="8">
         <v>5</v>
       </c>
-      <c r="E10" s="12">
-        <v>2</v>
-      </c>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+      <c r="E10" s="9">
+        <v>1</v>
+      </c>
+      <c r="F10" s="10">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G10" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="2:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C11" s="7"/>
-      <c r="D11" s="11">
+      <c r="C11" s="13"/>
+      <c r="D11" s="8">
         <v>6</v>
       </c>
-      <c r="E11" s="12">
-        <v>2</v>
-      </c>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
+      <c r="E11" s="9">
+        <v>1</v>
+      </c>
+      <c r="F11" s="10">
+        <v>1</v>
+      </c>
+      <c r="G11" s="10">
+        <v>0.9</v>
+      </c>
     </row>
     <row r="12" spans="2:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C12" s="7"/>
-      <c r="D12" s="11">
+      <c r="C12" s="13"/>
+      <c r="D12" s="8">
         <v>7</v>
       </c>
-      <c r="E12" s="12">
-        <v>1.5</v>
-      </c>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
+      <c r="E12" s="9">
+        <v>0.75</v>
+      </c>
+      <c r="F12" s="10">
+        <v>0.9</v>
+      </c>
+      <c r="G12" s="10">
+        <v>0.80000000000000104</v>
+      </c>
     </row>
     <row r="13" spans="2:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="C13" s="14"/>
-      <c r="D13" s="15">
+      <c r="D13" s="11">
         <v>8</v>
       </c>
-      <c r="E13" s="12">
-        <v>1.5</v>
-      </c>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
+      <c r="E13" s="9">
+        <v>0.75</v>
+      </c>
+      <c r="F13" s="10">
+        <v>0.75</v>
+      </c>
+      <c r="G13" s="10">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="14" spans="2:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="G14" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="15" spans="2:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C15" s="7"/>
-      <c r="D15" s="8">
+      <c r="C15" s="13"/>
+      <c r="D15" s="5">
         <v>1</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="6">
+        <v>5.5</v>
+      </c>
+      <c r="F15" s="7">
+        <v>4</v>
+      </c>
+      <c r="G15" s="7">
+        <v>3.5</v>
+      </c>
+      <c r="I15" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="C16" s="13"/>
+      <c r="D16" s="8">
+        <v>2</v>
+      </c>
+      <c r="E16" s="9">
+        <f>E15-1</f>
+        <v>4.5</v>
+      </c>
+      <c r="F16" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="G16" s="10">
+        <v>3</v>
+      </c>
+      <c r="I16" s="16"/>
+    </row>
+    <row r="17" spans="3:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="C17" s="13"/>
+      <c r="D17" s="8">
+        <v>3</v>
+      </c>
+      <c r="E17" s="9">
+        <f t="shared" ref="E17:E18" si="0">E16-1</f>
+        <v>3.5</v>
+      </c>
+      <c r="F17" s="10">
+        <v>3</v>
+      </c>
+      <c r="G17" s="10">
+        <v>2.5</v>
+      </c>
+      <c r="I17" s="16"/>
+    </row>
+    <row r="18" spans="3:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="C18" s="13"/>
+      <c r="D18" s="8">
+        <v>4</v>
+      </c>
+      <c r="E18" s="9">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="F18" s="10">
+        <v>2.5</v>
+      </c>
+      <c r="G18" s="10">
+        <v>2</v>
+      </c>
+      <c r="I18" s="16"/>
+    </row>
+    <row r="19" spans="3:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="C19" s="13"/>
+      <c r="D19" s="8">
         <v>5</v>
       </c>
-      <c r="F15" s="10">
+      <c r="E19" s="9"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+    </row>
+    <row r="20" spans="3:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="C20" s="13"/>
+      <c r="D20" s="8">
+        <v>6</v>
+      </c>
+      <c r="E20" s="9"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+    </row>
+    <row r="21" spans="3:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="C21" s="13"/>
+      <c r="D21" s="8">
+        <v>7</v>
+      </c>
+      <c r="E21" s="9"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+    </row>
+    <row r="22" spans="3:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="C22" s="14"/>
+      <c r="D22" s="11">
+        <v>8</v>
+      </c>
+      <c r="E22" s="9"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+    </row>
+    <row r="23" spans="3:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="C23" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="G15" s="10">
+      <c r="D23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="3:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="C24" s="13"/>
+      <c r="D24" s="5">
+        <v>1</v>
+      </c>
+      <c r="E24" s="6">
+        <f>E15</f>
+        <v>5.5</v>
+      </c>
+      <c r="F24" s="6">
+        <f t="shared" ref="F24:G24" si="1">F15</f>
+        <v>4</v>
+      </c>
+      <c r="G24" s="6">
+        <f t="shared" si="1"/>
         <v>3.5</v>
       </c>
     </row>
-    <row r="16" spans="2:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C16" s="7"/>
-      <c r="D16" s="11">
+    <row r="25" spans="3:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="C25" s="13"/>
+      <c r="D25" s="8">
         <v>2</v>
       </c>
-      <c r="E16" s="12"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-    </row>
-    <row r="17" spans="3:7" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C17" s="7"/>
-      <c r="D17" s="11">
+      <c r="E25" s="9"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+    </row>
+    <row r="26" spans="3:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="C26" s="13"/>
+      <c r="D26" s="8">
         <v>3</v>
       </c>
-      <c r="E17" s="12"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-    </row>
-    <row r="18" spans="3:7" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C18" s="7"/>
-      <c r="D18" s="11">
+      <c r="E26" s="9"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+    </row>
+    <row r="27" spans="3:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="C27" s="13"/>
+      <c r="D27" s="8">
         <v>4</v>
       </c>
-      <c r="E18" s="12"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-    </row>
-    <row r="19" spans="3:7" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C19" s="7"/>
-      <c r="D19" s="11">
+      <c r="E27" s="9"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+    </row>
+    <row r="28" spans="3:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="C28" s="13"/>
+      <c r="D28" s="8">
         <v>5</v>
       </c>
-      <c r="E19" s="12"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-    </row>
-    <row r="20" spans="3:7" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C20" s="7"/>
-      <c r="D20" s="11">
+      <c r="E28" s="9"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+    </row>
+    <row r="29" spans="3:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="C29" s="13"/>
+      <c r="D29" s="8">
         <v>6</v>
       </c>
-      <c r="E20" s="12"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-    </row>
-    <row r="21" spans="3:7" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C21" s="7"/>
-      <c r="D21" s="11">
+      <c r="E29" s="9"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+    </row>
+    <row r="30" spans="3:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="C30" s="13"/>
+      <c r="D30" s="8">
         <v>7</v>
       </c>
-      <c r="E21" s="12"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-    </row>
-    <row r="22" spans="3:7" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="C22" s="14"/>
-      <c r="D22" s="15">
+      <c r="E30" s="9"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+    </row>
+    <row r="31" spans="3:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="C31" s="14"/>
+      <c r="D31" s="11">
         <v>8</v>
       </c>
-      <c r="E22" s="12"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-    </row>
-    <row r="23" spans="3:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="C23" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G23" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="24" spans="3:7" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C24" s="7"/>
-      <c r="D24" s="8">
-        <v>1</v>
-      </c>
-      <c r="E24" s="9">
-        <f>E15</f>
-        <v>5</v>
-      </c>
-      <c r="F24" s="9">
-        <f t="shared" ref="F24:G24" si="0">F15</f>
-        <v>4</v>
-      </c>
-      <c r="G24" s="9">
-        <f t="shared" si="0"/>
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="25" spans="3:7" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C25" s="7"/>
-      <c r="D25" s="11">
-        <v>2</v>
-      </c>
-      <c r="E25" s="12"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-    </row>
-    <row r="26" spans="3:7" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C26" s="7"/>
-      <c r="D26" s="11">
-        <v>3</v>
-      </c>
-      <c r="E26" s="12"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-    </row>
-    <row r="27" spans="3:7" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C27" s="7"/>
-      <c r="D27" s="11">
-        <v>4</v>
-      </c>
-      <c r="E27" s="12"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-    </row>
-    <row r="28" spans="3:7" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C28" s="7"/>
-      <c r="D28" s="11">
-        <v>5</v>
-      </c>
-      <c r="E28" s="12"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-    </row>
-    <row r="29" spans="3:7" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C29" s="7"/>
-      <c r="D29" s="11">
-        <v>6</v>
-      </c>
-      <c r="E29" s="12"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-    </row>
-    <row r="30" spans="3:7" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C30" s="7"/>
-      <c r="D30" s="11">
-        <v>7</v>
-      </c>
-      <c r="E30" s="12"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-    </row>
-    <row r="31" spans="3:7" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="C31" s="14"/>
-      <c r="D31" s="15">
-        <v>8</v>
-      </c>
-      <c r="E31" s="12"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="C5:C13"/>
     <mergeCell ref="C14:C22"/>
     <mergeCell ref="C23:C31"/>
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="B3:I3"/>
+    <mergeCell ref="I15:I18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ran more cases with new Hughes Fix
</commit_message>
<xml_diff>
--- a/Opt_Test_Matrix.xlsx
+++ b/Opt_Test_Matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rthill\Documents\MS-Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FB7BEEE-CF77-4187-98A6-1A85BE4315C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20637048-8ED8-4FD3-9726-1F441B503346}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{ACE28608-3E68-4E86-80D4-7B51E677897B}"/>
   </bookViews>
@@ -836,8 +836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5177AB5A-2235-443C-BFC0-3BF5F1CC385F}">
   <dimension ref="B2:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -929,10 +929,10 @@
         <v>1.25</v>
       </c>
       <c r="F8" s="10">
-        <v>1.3</v>
+        <v>1.25</v>
       </c>
       <c r="G8" s="10">
-        <v>1.2</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="9" spans="2:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
@@ -944,10 +944,10 @@
         <v>1.25</v>
       </c>
       <c r="F9" s="10">
-        <v>1.2</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="G9" s="10">
-        <v>1.1000000000000001</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="10" spans="2:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
@@ -959,7 +959,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="10">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="G10" s="10">
         <v>1</v>
@@ -974,10 +974,10 @@
         <v>1</v>
       </c>
       <c r="F11" s="10">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="G11" s="10">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="12" spans="2:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
@@ -989,10 +989,10 @@
         <v>0.75</v>
       </c>
       <c r="F12" s="10">
-        <v>0.9</v>
+        <v>0.75</v>
       </c>
       <c r="G12" s="10">
-        <v>0.80000000000000104</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="13" spans="2:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
@@ -1004,10 +1004,10 @@
         <v>0.75</v>
       </c>
       <c r="F13" s="10">
-        <v>0.75</v>
+        <v>0.65</v>
       </c>
       <c r="G13" s="10">
-        <v>0.75</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.6">

</xml_diff>

<commit_message>
Setup iwo 10-08 meeting
</commit_message>
<xml_diff>
--- a/Opt_Test_Matrix.xlsx
+++ b/Opt_Test_Matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rthill\Documents\MS-Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20637048-8ED8-4FD3-9726-1F441B503346}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B47590-F70A-46D8-B760-6F017D92320B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{ACE28608-3E68-4E86-80D4-7B51E677897B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t xml:space="preserve">Structural Design Weight and Cost Tradeoffs for Attritable Vessels </t>
   </si>
@@ -146,14 +146,35 @@
     </r>
   </si>
   <si>
-    <t>*run these 4 cases first before continuing</t>
+    <t>*Current C1</t>
+  </si>
+  <si>
+    <t>*Current C2</t>
+  </si>
+  <si>
+    <t>*Current C3</t>
+  </si>
+  <si>
+    <t>*Current C4</t>
+  </si>
+  <si>
+    <t>Reliability-Based (RB) Smith collapse</t>
+  </si>
+  <si>
+    <t>*run first  case w/ Smith collapse</t>
+  </si>
+  <si>
+    <t>*re run all 8 cases w/ 200ind, 400gens, modified NSGA-II params</t>
+  </si>
+  <si>
+    <t>*run 3 more cases w/out smith collapse</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,6 +202,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF00B050"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -190,7 +230,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -353,11 +393,76 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -406,6 +511,60 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -428,16 +587,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>578224</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>147528</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>62753</xdr:rowOff>
+      <xdr:rowOff>39562</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>476090</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>45395</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>39820</xdr:rowOff>
+      <xdr:rowOff>16629</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -460,8 +619,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5952565" y="439271"/>
-          <a:ext cx="5025678" cy="1550373"/>
+          <a:off x="6442311" y="417249"/>
+          <a:ext cx="5013206" cy="1557389"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -834,18 +993,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5177AB5A-2235-443C-BFC0-3BF5F1CC385F}">
-  <dimension ref="B2:I31"/>
+  <dimension ref="B2:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AJ8" sqref="AJ8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="3" max="3" width="4.26171875" customWidth="1"/>
+    <col min="3" max="3" width="6.26171875" customWidth="1"/>
     <col min="5" max="5" width="10.68359375" customWidth="1"/>
     <col min="6" max="6" width="12.26171875" customWidth="1"/>
     <col min="7" max="7" width="11.578125" customWidth="1"/>
+    <col min="8" max="8" width="10.83984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="15.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -904,6 +1064,9 @@
       <c r="G6" s="7">
         <v>1.5</v>
       </c>
+      <c r="I6" s="28" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="7" spans="2:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="C7" s="13"/>
@@ -919,6 +1082,7 @@
       <c r="G7" s="10">
         <v>1.3</v>
       </c>
+      <c r="I7" s="28"/>
     </row>
     <row r="8" spans="2:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="C8" s="13"/>
@@ -934,6 +1098,7 @@
       <c r="G8" s="10">
         <v>1.25</v>
       </c>
+      <c r="I8" s="28"/>
     </row>
     <row r="9" spans="2:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="C9" s="13"/>
@@ -949,6 +1114,7 @@
       <c r="G9" s="10">
         <v>1.05</v>
       </c>
+      <c r="I9" s="28"/>
     </row>
     <row r="10" spans="2:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="C10" s="13"/>
@@ -964,6 +1130,7 @@
       <c r="G10" s="10">
         <v>1</v>
       </c>
+      <c r="I10" s="28"/>
     </row>
     <row r="11" spans="2:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="C11" s="13"/>
@@ -979,6 +1146,7 @@
       <c r="G11" s="10">
         <v>0.8</v>
       </c>
+      <c r="I11" s="28"/>
     </row>
     <row r="12" spans="2:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="C12" s="13"/>
@@ -994,6 +1162,7 @@
       <c r="G12" s="10">
         <v>0.75</v>
       </c>
+      <c r="I12" s="28"/>
     </row>
     <row r="13" spans="2:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="C13" s="14"/>
@@ -1027,22 +1196,25 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="2:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="2:9" ht="15.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="C15" s="13"/>
       <c r="D15" s="5">
         <v>1</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="17">
         <v>5.5</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="18">
         <v>4</v>
       </c>
-      <c r="G15" s="7">
+      <c r="G15" s="18">
         <v>3.5</v>
       </c>
-      <c r="I15" s="16" t="s">
+      <c r="H15" s="21" t="s">
         <v>12</v>
+      </c>
+      <c r="I15" s="28" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="2:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
@@ -1050,91 +1222,128 @@
       <c r="D16" s="8">
         <v>2</v>
       </c>
-      <c r="E16" s="9">
-        <f>E15-1</f>
-        <v>4.5</v>
-      </c>
-      <c r="F16" s="10">
-        <v>3.5</v>
-      </c>
-      <c r="G16" s="10">
-        <v>3</v>
-      </c>
-      <c r="I16" s="16"/>
+      <c r="E16" s="33">
+        <v>5</v>
+      </c>
+      <c r="F16" s="30">
+        <v>3.75</v>
+      </c>
+      <c r="G16" s="30">
+        <v>3.25</v>
+      </c>
+      <c r="H16" s="21"/>
+      <c r="I16" s="28"/>
     </row>
     <row r="17" spans="3:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="C17" s="13"/>
       <c r="D17" s="8">
         <v>3</v>
       </c>
-      <c r="E17" s="9">
-        <f t="shared" ref="E17:E18" si="0">E16-1</f>
+      <c r="E17" s="19">
+        <f>E15-1</f>
+        <v>4.5</v>
+      </c>
+      <c r="F17" s="20">
         <v>3.5</v>
       </c>
-      <c r="F17" s="10">
+      <c r="G17" s="20">
         <v>3</v>
       </c>
-      <c r="G17" s="10">
-        <v>2.5</v>
-      </c>
-      <c r="I17" s="16"/>
+      <c r="H17" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="I17" s="28"/>
     </row>
     <row r="18" spans="3:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="C18" s="13"/>
       <c r="D18" s="8">
         <v>4</v>
       </c>
-      <c r="E18" s="9">
-        <f t="shared" si="0"/>
-        <v>2.5</v>
-      </c>
-      <c r="F18" s="10">
-        <v>2.5</v>
-      </c>
-      <c r="G18" s="10">
-        <v>2</v>
-      </c>
-      <c r="I18" s="16"/>
+      <c r="E18" s="33">
+        <v>4</v>
+      </c>
+      <c r="F18" s="30">
+        <v>3.25</v>
+      </c>
+      <c r="G18" s="30">
+        <v>2.75</v>
+      </c>
+      <c r="H18" s="21"/>
+      <c r="I18" s="28"/>
     </row>
     <row r="19" spans="3:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="C19" s="13"/>
       <c r="D19" s="8">
         <v>5</v>
       </c>
-      <c r="E19" s="9"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
+      <c r="E19" s="19">
+        <f>E17-1</f>
+        <v>3.5</v>
+      </c>
+      <c r="F19" s="20">
+        <v>3</v>
+      </c>
+      <c r="G19" s="20">
+        <v>2.5</v>
+      </c>
+      <c r="H19" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="I19" s="28"/>
     </row>
     <row r="20" spans="3:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="C20" s="13"/>
       <c r="D20" s="8">
         <v>6</v>
       </c>
-      <c r="E20" s="9"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
+      <c r="E20" s="32">
+        <v>3</v>
+      </c>
+      <c r="F20" s="31">
+        <v>2.75</v>
+      </c>
+      <c r="G20" s="31">
+        <v>2.25</v>
+      </c>
+      <c r="H20" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20" s="28"/>
     </row>
     <row r="21" spans="3:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="C21" s="13"/>
       <c r="D21" s="8">
         <v>7</v>
       </c>
-      <c r="E21" s="9"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
+      <c r="E21" s="32">
+        <v>2.75</v>
+      </c>
+      <c r="F21" s="31">
+        <v>2.5</v>
+      </c>
+      <c r="G21" s="31">
+        <v>2</v>
+      </c>
+      <c r="H21" s="21"/>
     </row>
     <row r="22" spans="3:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
       <c r="C22" s="14"/>
       <c r="D22" s="11">
         <v>8</v>
       </c>
-      <c r="E22" s="9"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
+      <c r="E22" s="32">
+        <v>2.5</v>
+      </c>
+      <c r="F22" s="31">
+        <v>2.25</v>
+      </c>
+      <c r="G22" s="31">
+        <v>1.75</v>
+      </c>
     </row>
     <row r="23" spans="3:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.6">
       <c r="C23" s="12" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>5</v>
@@ -1149,22 +1358,22 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="3:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="3:9" ht="15.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="C24" s="13"/>
       <c r="D24" s="5">
         <v>1</v>
       </c>
-      <c r="E24" s="6">
-        <f>E15</f>
-        <v>5.5</v>
-      </c>
-      <c r="F24" s="6">
-        <f t="shared" ref="F24:G24" si="1">F15</f>
+      <c r="E24" s="34">
+        <v>5</v>
+      </c>
+      <c r="F24" s="29">
         <v>4</v>
       </c>
-      <c r="G24" s="6">
-        <f t="shared" si="1"/>
+      <c r="G24" s="29">
         <v>3.5</v>
+      </c>
+      <c r="I24" s="28" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="3:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
@@ -1172,45 +1381,50 @@
       <c r="D25" s="8">
         <v>2</v>
       </c>
-      <c r="E25" s="9"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="I25" s="28"/>
     </row>
     <row r="26" spans="3:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="C26" s="13"/>
       <c r="D26" s="8">
         <v>3</v>
       </c>
-      <c r="E26" s="9"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="I26" s="28"/>
     </row>
     <row r="27" spans="3:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="C27" s="13"/>
       <c r="D27" s="8">
         <v>4</v>
       </c>
-      <c r="E27" s="9"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="I27" s="28"/>
     </row>
     <row r="28" spans="3:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="C28" s="13"/>
       <c r="D28" s="8">
         <v>5</v>
       </c>
-      <c r="E28" s="9"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="I28" s="22"/>
     </row>
     <row r="29" spans="3:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="C29" s="13"/>
       <c r="D29" s="8">
         <v>6</v>
       </c>
-      <c r="E29" s="9"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
+      <c r="I29" s="22"/>
     </row>
     <row r="30" spans="3:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="C30" s="13"/>
@@ -1226,18 +1440,169 @@
       <c r="D31" s="11">
         <v>8</v>
       </c>
-      <c r="E31" s="9"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
+      <c r="E31" s="36"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
+    </row>
+    <row r="32" spans="3:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="C32" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="3:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="C33" s="26"/>
+      <c r="D33" s="5">
+        <v>1</v>
+      </c>
+      <c r="E33" s="17">
+        <v>5.5</v>
+      </c>
+      <c r="F33" s="18">
+        <v>4</v>
+      </c>
+      <c r="G33" s="18">
+        <v>3.5</v>
+      </c>
+      <c r="I33" s="16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="3:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="C34" s="26"/>
+      <c r="D34" s="8">
+        <v>2</v>
+      </c>
+      <c r="E34" s="33">
+        <v>5</v>
+      </c>
+      <c r="F34" s="30">
+        <v>3.75</v>
+      </c>
+      <c r="G34" s="30">
+        <v>3.25</v>
+      </c>
+      <c r="I34" s="16"/>
+    </row>
+    <row r="35" spans="3:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="C35" s="26"/>
+      <c r="D35" s="8">
+        <v>3</v>
+      </c>
+      <c r="E35" s="19">
+        <f>E33-1</f>
+        <v>4.5</v>
+      </c>
+      <c r="F35" s="20">
+        <v>3.5</v>
+      </c>
+      <c r="G35" s="20">
+        <v>3</v>
+      </c>
+      <c r="I35" s="16"/>
+    </row>
+    <row r="36" spans="3:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="C36" s="26"/>
+      <c r="D36" s="8">
+        <v>4</v>
+      </c>
+      <c r="E36" s="33">
+        <v>4</v>
+      </c>
+      <c r="F36" s="30">
+        <v>3.25</v>
+      </c>
+      <c r="G36" s="30">
+        <v>2.75</v>
+      </c>
+      <c r="I36" s="16"/>
+    </row>
+    <row r="37" spans="3:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="C37" s="26"/>
+      <c r="D37" s="8">
+        <v>5</v>
+      </c>
+      <c r="E37" s="19">
+        <f>E35-1</f>
+        <v>3.5</v>
+      </c>
+      <c r="F37" s="20">
+        <v>3</v>
+      </c>
+      <c r="G37" s="20">
+        <v>2.5</v>
+      </c>
+      <c r="I37" s="16"/>
+    </row>
+    <row r="38" spans="3:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="C38" s="26"/>
+      <c r="D38" s="8">
+        <v>6</v>
+      </c>
+      <c r="E38" s="32">
+        <v>3</v>
+      </c>
+      <c r="F38" s="31">
+        <v>2.75</v>
+      </c>
+      <c r="G38" s="31">
+        <v>2.25</v>
+      </c>
+      <c r="I38" s="16"/>
+    </row>
+    <row r="39" spans="3:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+      <c r="C39" s="26"/>
+      <c r="D39" s="8">
+        <v>7</v>
+      </c>
+      <c r="E39" s="32">
+        <v>2.75</v>
+      </c>
+      <c r="F39" s="31">
+        <v>2.5</v>
+      </c>
+      <c r="G39" s="31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="3:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="C40" s="27"/>
+      <c r="D40" s="8">
+        <v>8</v>
+      </c>
+      <c r="E40" s="32">
+        <v>2.5</v>
+      </c>
+      <c r="F40" s="31">
+        <v>2.25</v>
+      </c>
+      <c r="G40" s="31">
+        <v>1.75</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="10">
     <mergeCell ref="C5:C13"/>
     <mergeCell ref="C14:C22"/>
-    <mergeCell ref="C23:C31"/>
+    <mergeCell ref="C32:C40"/>
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="B3:I3"/>
-    <mergeCell ref="I15:I18"/>
+    <mergeCell ref="I15:I20"/>
+    <mergeCell ref="C23:C31"/>
+    <mergeCell ref="I24:I27"/>
+    <mergeCell ref="I33:I38"/>
+    <mergeCell ref="I6:I12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Corrected bounds, ready to re-run everything
</commit_message>
<xml_diff>
--- a/Opt_Test_Matrix.xlsx
+++ b/Opt_Test_Matrix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\Michigan Documents\First Term\Master's Thesis\Code\Working\MS-Thesis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rthill\Documents\MS-Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D99FB7-1306-4F22-A4FE-252DAD969851}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D26FE0EE-A952-4514-ABCE-E56184067E8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-4005" windowWidth="38640" windowHeight="21240" xr2:uid="{ACE28608-3E68-4E86-80D4-7B51E677897B}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{ACE28608-3E68-4E86-80D4-7B51E677897B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -230,7 +230,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -420,49 +420,25 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -513,13 +489,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -530,10 +502,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -989,8 +957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5177AB5A-2235-443C-BFC0-3BF5F1CC385F}">
   <dimension ref="B2:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1003,32 +971,32 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="15.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
     </row>
     <row r="3" spans="2:9" ht="15.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
     </row>
     <row r="4" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="5" spans="2:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="23" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -1045,7 +1013,7 @@
       </c>
     </row>
     <row r="6" spans="2:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C6" s="28"/>
+      <c r="C6" s="24"/>
       <c r="D6" s="5">
         <v>1</v>
       </c>
@@ -1058,12 +1026,12 @@
       <c r="G6" s="7">
         <v>1.5</v>
       </c>
-      <c r="I6" s="33" t="s">
+      <c r="I6" s="29" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C7" s="28"/>
+      <c r="C7" s="24"/>
       <c r="D7" s="8">
         <v>2</v>
       </c>
@@ -1076,10 +1044,10 @@
       <c r="G7" s="10">
         <v>1.3</v>
       </c>
-      <c r="I7" s="33"/>
+      <c r="I7" s="29"/>
     </row>
     <row r="8" spans="2:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C8" s="28"/>
+      <c r="C8" s="24"/>
       <c r="D8" s="8">
         <v>3</v>
       </c>
@@ -1092,10 +1060,10 @@
       <c r="G8" s="10">
         <v>1.25</v>
       </c>
-      <c r="I8" s="33"/>
+      <c r="I8" s="29"/>
     </row>
     <row r="9" spans="2:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C9" s="28"/>
+      <c r="C9" s="24"/>
       <c r="D9" s="8">
         <v>4</v>
       </c>
@@ -1108,10 +1076,10 @@
       <c r="G9" s="10">
         <v>1.05</v>
       </c>
-      <c r="I9" s="33"/>
+      <c r="I9" s="29"/>
     </row>
     <row r="10" spans="2:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C10" s="28"/>
+      <c r="C10" s="24"/>
       <c r="D10" s="8">
         <v>5</v>
       </c>
@@ -1124,10 +1092,10 @@
       <c r="G10" s="10">
         <v>1</v>
       </c>
-      <c r="I10" s="33"/>
+      <c r="I10" s="29"/>
     </row>
     <row r="11" spans="2:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C11" s="28"/>
+      <c r="C11" s="24"/>
       <c r="D11" s="8">
         <v>6</v>
       </c>
@@ -1140,10 +1108,10 @@
       <c r="G11" s="10">
         <v>0.8</v>
       </c>
-      <c r="I11" s="33"/>
+      <c r="I11" s="29"/>
     </row>
     <row r="12" spans="2:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C12" s="28"/>
+      <c r="C12" s="24"/>
       <c r="D12" s="8">
         <v>7</v>
       </c>
@@ -1156,10 +1124,10 @@
       <c r="G12" s="10">
         <v>0.75</v>
       </c>
-      <c r="I12" s="33"/>
+      <c r="I12" s="29"/>
     </row>
     <row r="13" spans="2:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="C13" s="29"/>
+      <c r="C13" s="25"/>
       <c r="D13" s="11">
         <v>8</v>
       </c>
@@ -1174,7 +1142,7 @@
       </c>
     </row>
     <row r="14" spans="2:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="C14" s="27" t="s">
+      <c r="C14" s="23" t="s">
         <v>3</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -1191,7 +1159,7 @@
       </c>
     </row>
     <row r="15" spans="2:9" ht="15.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C15" s="28"/>
+      <c r="C15" s="24"/>
       <c r="D15" s="5">
         <v>1</v>
       </c>
@@ -1207,29 +1175,29 @@
       <c r="H15" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="I15" s="33" t="s">
+      <c r="I15" s="29" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="16" spans="2:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C16" s="28"/>
+      <c r="C16" s="24"/>
       <c r="D16" s="8">
         <v>2</v>
       </c>
-      <c r="E16" s="23">
+      <c r="E16" s="21">
         <v>5</v>
       </c>
-      <c r="F16" s="22">
+      <c r="F16" s="20">
         <v>3.75</v>
       </c>
-      <c r="G16" s="22">
+      <c r="G16" s="20">
         <v>3.25</v>
       </c>
       <c r="H16" s="16"/>
-      <c r="I16" s="33"/>
+      <c r="I16" s="29"/>
     </row>
     <row r="17" spans="3:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C17" s="28"/>
+      <c r="C17" s="24"/>
       <c r="D17" s="8">
         <v>3</v>
       </c>
@@ -1246,27 +1214,27 @@
       <c r="H17" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="I17" s="33"/>
+      <c r="I17" s="29"/>
     </row>
     <row r="18" spans="3:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C18" s="28"/>
+      <c r="C18" s="24"/>
       <c r="D18" s="8">
         <v>4</v>
       </c>
-      <c r="E18" s="23">
+      <c r="E18" s="21">
         <v>4</v>
       </c>
-      <c r="F18" s="22">
+      <c r="F18" s="20">
         <v>3.25</v>
       </c>
-      <c r="G18" s="22">
+      <c r="G18" s="20">
         <v>2.75</v>
       </c>
       <c r="H18" s="16"/>
-      <c r="I18" s="33"/>
+      <c r="I18" s="29"/>
     </row>
     <row r="19" spans="3:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C19" s="28"/>
+      <c r="C19" s="24"/>
       <c r="D19" s="8">
         <v>5</v>
       </c>
@@ -1283,60 +1251,60 @@
       <c r="H19" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="I19" s="33"/>
+      <c r="I19" s="29"/>
     </row>
     <row r="20" spans="3:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C20" s="28"/>
+      <c r="C20" s="24"/>
       <c r="D20" s="8">
         <v>6</v>
       </c>
-      <c r="E20" s="23">
+      <c r="E20" s="21">
         <v>3</v>
       </c>
-      <c r="F20" s="22">
+      <c r="F20" s="20">
         <v>2.75</v>
       </c>
-      <c r="G20" s="22">
+      <c r="G20" s="20">
         <v>2.25</v>
       </c>
       <c r="H20" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="I20" s="33"/>
+      <c r="I20" s="29"/>
     </row>
     <row r="21" spans="3:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C21" s="28"/>
+      <c r="C21" s="24"/>
       <c r="D21" s="8">
         <v>7</v>
       </c>
-      <c r="E21" s="23">
+      <c r="E21" s="21">
         <v>2.75</v>
       </c>
-      <c r="F21" s="22">
+      <c r="F21" s="20">
         <v>2.5</v>
       </c>
-      <c r="G21" s="22">
+      <c r="G21" s="20">
         <v>2</v>
       </c>
       <c r="H21" s="16"/>
     </row>
     <row r="22" spans="3:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="C22" s="29"/>
+      <c r="C22" s="25"/>
       <c r="D22" s="11">
         <v>8</v>
       </c>
-      <c r="E22" s="23">
+      <c r="E22" s="21">
         <v>2.5</v>
       </c>
-      <c r="F22" s="22">
+      <c r="F22" s="20">
         <v>2.25</v>
       </c>
-      <c r="G22" s="22">
+      <c r="G22" s="20">
         <v>1.75</v>
       </c>
     </row>
     <row r="23" spans="3:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="C23" s="27" t="s">
+      <c r="C23" s="23" t="s">
         <v>16</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -1353,99 +1321,141 @@
       </c>
     </row>
     <row r="24" spans="3:9" ht="15.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C24" s="28"/>
+      <c r="C24" s="24"/>
       <c r="D24" s="5">
         <v>1</v>
       </c>
-      <c r="E24" s="24">
+      <c r="E24" s="22">
         <v>5</v>
       </c>
-      <c r="F24" s="21">
+      <c r="F24" s="19">
         <v>4</v>
       </c>
-      <c r="G24" s="21">
+      <c r="G24" s="19">
         <v>3.5</v>
       </c>
-      <c r="I24" s="33" t="s">
+      <c r="I24" s="29" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="25" spans="3:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C25" s="28"/>
+      <c r="C25" s="24"/>
       <c r="D25" s="8">
         <v>2</v>
       </c>
-      <c r="E25" s="14"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="I25" s="33"/>
+      <c r="E25" s="21">
+        <v>4.5</v>
+      </c>
+      <c r="F25" s="20">
+        <v>3.75</v>
+      </c>
+      <c r="G25" s="20">
+        <v>3.25</v>
+      </c>
+      <c r="I25" s="29"/>
     </row>
     <row r="26" spans="3:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C26" s="28"/>
+      <c r="C26" s="24"/>
       <c r="D26" s="8">
         <v>3</v>
       </c>
-      <c r="E26" s="14"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
-      <c r="I26" s="33"/>
+      <c r="E26" s="21">
+        <v>4</v>
+      </c>
+      <c r="F26" s="20">
+        <v>3.5</v>
+      </c>
+      <c r="G26" s="20">
+        <v>3</v>
+      </c>
+      <c r="I26" s="29"/>
     </row>
     <row r="27" spans="3:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C27" s="28"/>
+      <c r="C27" s="24"/>
       <c r="D27" s="8">
         <v>4</v>
       </c>
-      <c r="E27" s="14"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
-      <c r="I27" s="33"/>
+      <c r="E27" s="21">
+        <v>3.5</v>
+      </c>
+      <c r="F27" s="20">
+        <v>3.25</v>
+      </c>
+      <c r="G27" s="20">
+        <v>2.75</v>
+      </c>
+      <c r="I27" s="29"/>
     </row>
     <row r="28" spans="3:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C28" s="28"/>
+      <c r="C28" s="24"/>
       <c r="D28" s="8">
         <v>5</v>
       </c>
-      <c r="E28" s="25"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
+      <c r="E28" s="21">
+        <v>3.25</v>
+      </c>
+      <c r="F28" s="21">
+        <v>3</v>
+      </c>
+      <c r="G28" s="21">
+        <v>2.5</v>
+      </c>
       <c r="I28" s="17"/>
     </row>
     <row r="29" spans="3:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C29" s="28"/>
+      <c r="C29" s="24"/>
       <c r="D29" s="8">
         <v>6</v>
       </c>
-      <c r="E29" s="25"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
+      <c r="E29" s="21">
+        <v>3</v>
+      </c>
+      <c r="F29" s="21">
+        <v>2.75</v>
+      </c>
+      <c r="G29" s="21">
+        <v>2.25</v>
+      </c>
       <c r="I29" s="17"/>
     </row>
     <row r="30" spans="3:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C30" s="28"/>
+      <c r="C30" s="24"/>
       <c r="D30" s="8">
         <v>7</v>
       </c>
-      <c r="E30" s="9"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
+      <c r="E30" s="21">
+        <v>2.75</v>
+      </c>
+      <c r="F30" s="21">
+        <v>2.5</v>
+      </c>
+      <c r="G30" s="21">
+        <v>2</v>
+      </c>
     </row>
     <row r="31" spans="3:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="C31" s="29"/>
+      <c r="C31" s="25"/>
       <c r="D31" s="11">
         <v>8</v>
       </c>
-      <c r="E31" s="26"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
+      <c r="E31" s="21">
+        <v>2.5</v>
+      </c>
+      <c r="F31" s="21">
+        <v>2.25</v>
+      </c>
+      <c r="G31" s="21">
+        <v>1.75</v>
+      </c>
     </row>
     <row r="32" spans="3:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="C32" s="27" t="s">
+      <c r="C32" s="23" t="s">
         <v>4</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E32" s="20" t="s">
+      <c r="E32" s="18" t="s">
         <v>9</v>
       </c>
       <c r="F32" s="3" t="s">
@@ -1456,7 +1466,7 @@
       </c>
     </row>
     <row r="33" spans="3:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C33" s="30"/>
+      <c r="C33" s="26"/>
       <c r="D33" s="5">
         <v>1</v>
       </c>
@@ -1469,28 +1479,28 @@
       <c r="G33" s="13">
         <v>3.5</v>
       </c>
-      <c r="I33" s="34" t="s">
+      <c r="I33" s="30" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="34" spans="3:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C34" s="30"/>
+      <c r="C34" s="26"/>
       <c r="D34" s="8">
         <v>2</v>
       </c>
-      <c r="E34" s="23">
+      <c r="E34" s="21">
         <v>5</v>
       </c>
-      <c r="F34" s="22">
+      <c r="F34" s="20">
         <v>3.75</v>
       </c>
-      <c r="G34" s="22">
+      <c r="G34" s="20">
         <v>3.25</v>
       </c>
-      <c r="I34" s="34"/>
+      <c r="I34" s="30"/>
     </row>
     <row r="35" spans="3:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C35" s="30"/>
+      <c r="C35" s="26"/>
       <c r="D35" s="8">
         <v>3</v>
       </c>
@@ -1504,26 +1514,26 @@
       <c r="G35" s="15">
         <v>3</v>
       </c>
-      <c r="I35" s="34"/>
+      <c r="I35" s="30"/>
     </row>
     <row r="36" spans="3:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C36" s="30"/>
+      <c r="C36" s="26"/>
       <c r="D36" s="8">
         <v>4</v>
       </c>
-      <c r="E36" s="23">
+      <c r="E36" s="21">
         <v>4</v>
       </c>
-      <c r="F36" s="22">
+      <c r="F36" s="20">
         <v>3.25</v>
       </c>
-      <c r="G36" s="22">
+      <c r="G36" s="20">
         <v>2.75</v>
       </c>
-      <c r="I36" s="34"/>
+      <c r="I36" s="30"/>
     </row>
     <row r="37" spans="3:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C37" s="30"/>
+      <c r="C37" s="26"/>
       <c r="D37" s="8">
         <v>5</v>
       </c>
@@ -1537,51 +1547,51 @@
       <c r="G37" s="15">
         <v>2.5</v>
       </c>
-      <c r="I37" s="34"/>
+      <c r="I37" s="30"/>
     </row>
     <row r="38" spans="3:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C38" s="30"/>
+      <c r="C38" s="26"/>
       <c r="D38" s="8">
         <v>6</v>
       </c>
-      <c r="E38" s="23">
+      <c r="E38" s="21">
         <v>3</v>
       </c>
-      <c r="F38" s="22">
+      <c r="F38" s="20">
         <v>2.75</v>
       </c>
-      <c r="G38" s="22">
+      <c r="G38" s="20">
         <v>2.25</v>
       </c>
-      <c r="I38" s="34"/>
+      <c r="I38" s="30"/>
     </row>
     <row r="39" spans="3:9" ht="15.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C39" s="30"/>
+      <c r="C39" s="26"/>
       <c r="D39" s="8">
         <v>7</v>
       </c>
-      <c r="E39" s="23">
+      <c r="E39" s="21">
         <v>2.75</v>
       </c>
-      <c r="F39" s="22">
+      <c r="F39" s="20">
         <v>2.5</v>
       </c>
-      <c r="G39" s="22">
+      <c r="G39" s="20">
         <v>2</v>
       </c>
     </row>
     <row r="40" spans="3:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="C40" s="31"/>
+      <c r="C40" s="27"/>
       <c r="D40" s="8">
         <v>8</v>
       </c>
-      <c r="E40" s="23">
+      <c r="E40" s="21">
         <v>2.5</v>
       </c>
-      <c r="F40" s="22">
+      <c r="F40" s="20">
         <v>2.25</v>
       </c>
-      <c r="G40" s="22">
+      <c r="G40" s="20">
         <v>1.75</v>
       </c>
     </row>

</xml_diff>